<commit_message>
finished implementing step function on biomarkers
</commit_message>
<xml_diff>
--- a/data/cleaned/Compound annotation updated.xlsx
+++ b/data/cleaned/Compound annotation updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottericr/Documents/Tufts/Research Projects/2017 - 2018 Leafhopper Density/data/cleaned/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393F9A0A-1DC3-8440-815C-6B062AAD6DD6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A4F2C2-8ED8-494C-89CC-87A709BBCC20}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="0" windowWidth="25600" windowHeight="20480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25580" yWindow="460" windowWidth="25600" windowHeight="18680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compound annotation updated" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4244" uniqueCount="1333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4243" uniqueCount="1336">
   <si>
     <t>Compound</t>
   </si>
@@ -4020,13 +4020,22 @@
   </si>
   <si>
     <t>Reported as major biomarker of leafhopper damage on tea by Zeng et al. 2018 (doi: 10.1080/10408398.2018.1506907).  Precursor to hotrienol, which is formed durring dehydration and heating durring processing.</t>
+  </si>
+  <si>
+    <t>cis-Linalool oxide (pyranoid)</t>
+  </si>
+  <si>
+    <t>fungicide used in citrus farming</t>
+  </si>
+  <si>
+    <t>Aromatic compound</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4160,6 +4169,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -4503,12 +4518,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4866,8 +4882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O333"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5350,7 +5366,7 @@
         <v>17</v>
       </c>
       <c r="I11" t="s">
-        <v>17</v>
+        <v>1324</v>
       </c>
       <c r="J11" t="s">
         <v>17</v>
@@ -5368,7 +5384,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -5393,9 +5409,7 @@
       <c r="H12" t="s">
         <v>55</v>
       </c>
-      <c r="I12" t="s">
-        <v>17</v>
-      </c>
+      <c r="I12" s="3"/>
       <c r="J12" t="s">
         <v>17</v>
       </c>
@@ -5834,7 +5848,7 @@
         <v>17</v>
       </c>
       <c r="I22" t="s">
-        <v>17</v>
+        <v>319</v>
       </c>
       <c r="J22" t="s">
         <v>17</v>
@@ -6588,7 +6602,7 @@
         <v>185</v>
       </c>
       <c r="I39" t="s">
-        <v>17</v>
+        <v>1319</v>
       </c>
       <c r="J39" t="s">
         <v>17</v>
@@ -6632,7 +6646,7 @@
         <v>189</v>
       </c>
       <c r="I40" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="J40" t="s">
         <v>17</v>
@@ -7738,7 +7752,7 @@
         <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>311</v>
+        <v>1333</v>
       </c>
       <c r="F65" t="s">
         <v>17</v>
@@ -8096,13 +8110,13 @@
         <v>354</v>
       </c>
       <c r="G73" t="s">
-        <v>17</v>
+        <v>1334</v>
       </c>
       <c r="H73" t="s">
         <v>17</v>
       </c>
       <c r="I73" t="s">
-        <v>17</v>
+        <v>1335</v>
       </c>
       <c r="J73" t="s">
         <v>17</v>
@@ -19574,5 +19588,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made changes to biomarker table, ignore step function if CI of changepoint includes zero.
</commit_message>
<xml_diff>
--- a/data/cleaned/Compound annotation updated.xlsx
+++ b/data/cleaned/Compound annotation updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottericr/Documents/Tufts/Research Projects/2017 - 2018 Leafhopper Density/data/cleaned/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A4F2C2-8ED8-494C-89CC-87A709BBCC20}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCECA3B-918D-B545-93DC-E0F096FA341D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25580" yWindow="460" windowWidth="25600" windowHeight="18680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compound annotation updated" sheetId="1" r:id="rId1"/>
@@ -4883,7 +4883,7 @@
   <dimension ref="A1:O333"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+      <selection activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6646,7 +6646,7 @@
         <v>189</v>
       </c>
       <c r="I40" t="s">
-        <v>65</v>
+        <v>319</v>
       </c>
       <c r="J40" t="s">
         <v>17</v>
@@ -6778,7 +6778,7 @@
         <v>203</v>
       </c>
       <c r="I43" t="s">
-        <v>17</v>
+        <v>1320</v>
       </c>
       <c r="J43" t="s">
         <v>17</v>
@@ -7764,7 +7764,7 @@
         <v>312</v>
       </c>
       <c r="I65" t="s">
-        <v>17</v>
+        <v>319</v>
       </c>
       <c r="J65" t="s">
         <v>17</v>
@@ -8694,7 +8694,7 @@
         <v>17</v>
       </c>
       <c r="I86" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
       <c r="J86" t="s">
         <v>17</v>
@@ -9046,7 +9046,7 @@
         <v>189</v>
       </c>
       <c r="I94" t="s">
-        <v>17</v>
+        <v>319</v>
       </c>
       <c r="J94" t="s">
         <v>17</v>
@@ -17538,7 +17538,7 @@
         <v>17</v>
       </c>
       <c r="I287" t="s">
-        <v>17</v>
+        <v>319</v>
       </c>
       <c r="J287" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
made supplemental table 2 (2018 data) and updated lit RIs
</commit_message>
<xml_diff>
--- a/data/cleaned/Compound annotation updated.xlsx
+++ b/data/cleaned/Compound annotation updated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottericr/Documents/Tufts/Research Projects/2017 - 2018 Leafhopper Density/data/cleaned/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B896BF72-0265-644D-835B-E639E1BA0664}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C325B9C-4832-6F44-809B-55EF4F758847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-2020" windowWidth="25600" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compound annotation updated" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4273" uniqueCount="1349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4222" uniqueCount="1349">
   <si>
     <t>Compound</t>
   </si>
@@ -4928,8 +4928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="M163" sqref="M163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5423,11 +5423,11 @@
       <c r="L11" t="s">
         <v>17</v>
       </c>
-      <c r="M11" t="s">
-        <v>17</v>
+      <c r="M11">
+        <v>853</v>
       </c>
       <c r="N11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="23" x14ac:dyDescent="0.3">
@@ -5465,11 +5465,11 @@
       <c r="L12" t="s">
         <v>17</v>
       </c>
-      <c r="M12" t="s">
-        <v>17</v>
+      <c r="M12">
+        <v>926</v>
       </c>
       <c r="N12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -5685,11 +5685,11 @@
       <c r="L17" t="s">
         <v>17</v>
       </c>
-      <c r="M17" t="s">
-        <v>17</v>
+      <c r="M17">
+        <v>989</v>
       </c>
       <c r="N17" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -7143,11 +7143,11 @@
       <c r="L50" t="s">
         <v>17</v>
       </c>
-      <c r="M50" t="s">
-        <v>17</v>
+      <c r="M50">
+        <v>1310</v>
       </c>
       <c r="N50" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
@@ -7319,11 +7319,11 @@
       <c r="L54" t="s">
         <v>17</v>
       </c>
-      <c r="M54" t="s">
-        <v>17</v>
+      <c r="M54">
+        <v>1023</v>
       </c>
       <c r="N54" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
@@ -8255,11 +8255,11 @@
       <c r="L75" t="s">
         <v>17</v>
       </c>
-      <c r="M75" t="s">
-        <v>17</v>
+      <c r="M75">
+        <v>1510</v>
       </c>
       <c r="N75" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
@@ -8657,11 +8657,11 @@
       <c r="L84" t="s">
         <v>17</v>
       </c>
-      <c r="M84" t="s">
-        <v>17</v>
+      <c r="M84">
+        <v>946</v>
       </c>
       <c r="N84" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
@@ -9405,11 +9405,11 @@
       <c r="L101" t="s">
         <v>17</v>
       </c>
-      <c r="M101" t="s">
-        <v>17</v>
+      <c r="M101">
+        <v>1182</v>
       </c>
       <c r="N101" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
@@ -9493,11 +9493,11 @@
       <c r="L103" t="s">
         <v>17</v>
       </c>
-      <c r="M103" t="s">
-        <v>17</v>
+      <c r="M103">
+        <v>1021</v>
       </c>
       <c r="N103" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
@@ -9625,11 +9625,11 @@
       <c r="L106" t="s">
         <v>17</v>
       </c>
-      <c r="M106" t="s">
-        <v>17</v>
+      <c r="M106">
+        <v>1436</v>
       </c>
       <c r="N106" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
@@ -10945,11 +10945,11 @@
       <c r="L136" t="s">
         <v>17</v>
       </c>
-      <c r="M136" t="s">
-        <v>17</v>
+      <c r="M136">
+        <v>758</v>
       </c>
       <c r="N136" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.2">
@@ -10989,11 +10989,11 @@
       <c r="L137" t="s">
         <v>17</v>
       </c>
-      <c r="M137" t="s">
-        <v>17</v>
+      <c r="M137">
+        <v>883</v>
       </c>
       <c r="N137" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
@@ -11121,11 +11121,11 @@
       <c r="L140" t="s">
         <v>17</v>
       </c>
-      <c r="M140" t="s">
-        <v>17</v>
+      <c r="M140">
+        <v>1045</v>
       </c>
       <c r="N140" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
@@ -11209,11 +11209,11 @@
       <c r="L142" t="s">
         <v>17</v>
       </c>
-      <c r="M142" t="s">
-        <v>17</v>
+      <c r="M142">
+        <v>793</v>
       </c>
       <c r="N142" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
@@ -11473,11 +11473,11 @@
       <c r="L148" t="s">
         <v>17</v>
       </c>
-      <c r="M148" t="s">
-        <v>17</v>
+      <c r="M148">
+        <v>843</v>
       </c>
       <c r="N148" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
@@ -11561,11 +11561,11 @@
       <c r="L150" t="s">
         <v>17</v>
       </c>
-      <c r="M150" t="s">
-        <v>17</v>
+      <c r="M150">
+        <v>966</v>
       </c>
       <c r="N150" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.2">
@@ -11869,11 +11869,11 @@
       <c r="L157" t="s">
         <v>17</v>
       </c>
-      <c r="M157" t="s">
-        <v>17</v>
+      <c r="M157">
+        <v>815</v>
       </c>
       <c r="N157" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
@@ -11957,11 +11957,11 @@
       <c r="L159" t="s">
         <v>17</v>
       </c>
-      <c r="M159" t="s">
-        <v>17</v>
+      <c r="M159">
+        <v>981</v>
       </c>
       <c r="N159" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
@@ -12089,11 +12089,11 @@
       <c r="L162" t="s">
         <v>17</v>
       </c>
-      <c r="M162" t="s">
-        <v>17</v>
+      <c r="M162">
+        <v>1774</v>
       </c>
       <c r="N162" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.2">
@@ -12221,11 +12221,11 @@
       <c r="L165" t="s">
         <v>17</v>
       </c>
-      <c r="M165" t="s">
-        <v>17</v>
+      <c r="M165">
+        <v>1492</v>
       </c>
       <c r="N165" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.2">
@@ -13497,11 +13497,11 @@
       <c r="L194" t="s">
         <v>17</v>
       </c>
-      <c r="M194" t="s">
-        <v>17</v>
+      <c r="M194">
+        <v>1308</v>
       </c>
       <c r="N194" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="195" spans="1:14" x14ac:dyDescent="0.2">
@@ -13629,11 +13629,11 @@
       <c r="L197" t="s">
         <v>17</v>
       </c>
-      <c r="M197" t="s">
-        <v>17</v>
+      <c r="M197">
+        <v>960</v>
       </c>
       <c r="N197" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="198" spans="1:14" x14ac:dyDescent="0.2">
@@ -13673,11 +13673,11 @@
       <c r="L198" t="s">
         <v>17</v>
       </c>
-      <c r="M198" t="s">
-        <v>17</v>
+      <c r="M198">
+        <v>1121</v>
       </c>
       <c r="N198" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="199" spans="1:14" x14ac:dyDescent="0.2">
@@ -13761,11 +13761,11 @@
       <c r="L200" t="s">
         <v>17</v>
       </c>
-      <c r="M200" t="s">
-        <v>17</v>
+      <c r="M200">
+        <v>1080</v>
       </c>
       <c r="N200" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="201" spans="1:14" x14ac:dyDescent="0.2">
@@ -13893,11 +13893,11 @@
       <c r="L203" t="s">
         <v>17</v>
       </c>
-      <c r="M203" t="s">
-        <v>17</v>
+      <c r="M203">
+        <v>1094</v>
       </c>
       <c r="N203" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="204" spans="1:14" x14ac:dyDescent="0.2">
@@ -13981,11 +13981,11 @@
       <c r="L205" t="s">
         <v>17</v>
       </c>
-      <c r="M205" t="s">
-        <v>17</v>
+      <c r="M205">
+        <v>1735</v>
       </c>
       <c r="N205" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="206" spans="1:14" x14ac:dyDescent="0.2">
@@ -14377,8 +14377,8 @@
       <c r="L214" t="s">
         <v>17</v>
       </c>
-      <c r="M214" t="s">
-        <v>17</v>
+      <c r="M214">
+        <v>1377</v>
       </c>
       <c r="N214" t="s">
         <v>17</v>
@@ -14465,11 +14465,11 @@
       <c r="L216" t="s">
         <v>17</v>
       </c>
-      <c r="M216" t="s">
-        <v>17</v>
+      <c r="M216">
+        <v>909</v>
       </c>
       <c r="N216" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="217" spans="1:14" x14ac:dyDescent="0.2">
@@ -14905,11 +14905,11 @@
       <c r="L226" t="s">
         <v>17</v>
       </c>
-      <c r="M226" t="s">
-        <v>17</v>
+      <c r="M226">
+        <v>1531</v>
       </c>
       <c r="N226" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="227" spans="1:14" x14ac:dyDescent="0.2">
@@ -14993,11 +14993,11 @@
       <c r="L228" t="s">
         <v>17</v>
       </c>
-      <c r="M228" t="s">
-        <v>17</v>
+      <c r="M228">
+        <v>1253</v>
       </c>
       <c r="N228" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="229" spans="1:14" x14ac:dyDescent="0.2">
@@ -15389,8 +15389,8 @@
       <c r="L237" t="s">
         <v>17</v>
       </c>
-      <c r="M237" t="s">
-        <v>17</v>
+      <c r="M237">
+        <v>923</v>
       </c>
       <c r="N237" t="s">
         <v>17</v>
@@ -15521,11 +15521,11 @@
       <c r="L240" t="s">
         <v>17</v>
       </c>
-      <c r="M240" t="s">
-        <v>17</v>
+      <c r="M240">
+        <v>843</v>
       </c>
       <c r="N240" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="241" spans="1:14" x14ac:dyDescent="0.2">
@@ -15741,11 +15741,11 @@
       <c r="L245" t="s">
         <v>17</v>
       </c>
-      <c r="M245" t="s">
-        <v>17</v>
+      <c r="M245">
+        <v>1060</v>
       </c>
       <c r="N245" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="246" spans="1:14" x14ac:dyDescent="0.2">
@@ -16181,11 +16181,11 @@
       <c r="L255" t="s">
         <v>17</v>
       </c>
-      <c r="M255" t="s">
-        <v>17</v>
+      <c r="M255">
+        <v>1159</v>
       </c>
       <c r="N255" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="256" spans="1:14" x14ac:dyDescent="0.2">
@@ -16357,11 +16357,11 @@
       <c r="L259" t="s">
         <v>17</v>
       </c>
-      <c r="M259" t="s">
-        <v>17</v>
+      <c r="M259">
+        <v>1096</v>
       </c>
       <c r="N259" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="260" spans="1:14" x14ac:dyDescent="0.2">
@@ -16445,11 +16445,11 @@
       <c r="L261" t="s">
         <v>17</v>
       </c>
-      <c r="M261" t="s">
-        <v>17</v>
+      <c r="M261">
+        <v>921</v>
       </c>
       <c r="N261" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="262" spans="1:14" x14ac:dyDescent="0.2">
@@ -16665,11 +16665,11 @@
       <c r="L266" t="s">
         <v>17</v>
       </c>
-      <c r="M266" t="s">
-        <v>17</v>
+      <c r="M266">
+        <v>959</v>
       </c>
       <c r="N266" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="267" spans="1:14" x14ac:dyDescent="0.2">
@@ -16753,11 +16753,11 @@
       <c r="L268" t="s">
         <v>17</v>
       </c>
-      <c r="M268" t="s">
-        <v>17</v>
+      <c r="M268">
+        <v>1355</v>
       </c>
       <c r="N268" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="269" spans="1:14" x14ac:dyDescent="0.2">
@@ -16841,11 +16841,11 @@
       <c r="L270" t="s">
         <v>17</v>
       </c>
-      <c r="M270" t="s">
-        <v>17</v>
+      <c r="M270">
+        <v>1302</v>
       </c>
       <c r="N270" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="271" spans="1:14" x14ac:dyDescent="0.2">
@@ -16973,11 +16973,11 @@
       <c r="L273" t="s">
         <v>17</v>
       </c>
-      <c r="M273" t="s">
-        <v>17</v>
+      <c r="M273">
+        <v>1172</v>
       </c>
       <c r="N273" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="274" spans="1:14" x14ac:dyDescent="0.2">
@@ -17061,11 +17061,11 @@
       <c r="L275" t="s">
         <v>17</v>
       </c>
-      <c r="M275" t="s">
-        <v>17</v>
+      <c r="M275">
+        <v>777</v>
       </c>
       <c r="N275" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="276" spans="1:14" x14ac:dyDescent="0.2">
@@ -17193,11 +17193,11 @@
       <c r="L278" t="s">
         <v>17</v>
       </c>
-      <c r="M278" t="s">
-        <v>17</v>
+      <c r="M278">
+        <v>856</v>
       </c>
       <c r="N278" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="279" spans="1:14" x14ac:dyDescent="0.2">
@@ -17237,11 +17237,11 @@
       <c r="L279" t="s">
         <v>17</v>
       </c>
-      <c r="M279" t="s">
-        <v>17</v>
+      <c r="M279">
+        <v>1583</v>
       </c>
       <c r="N279" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="280" spans="1:14" x14ac:dyDescent="0.2">
@@ -17325,8 +17325,8 @@
       <c r="L281" t="s">
         <v>17</v>
       </c>
-      <c r="M281" t="s">
-        <v>17</v>
+      <c r="M281">
+        <v>1045</v>
       </c>
       <c r="N281" t="s">
         <v>17</v>
@@ -17853,11 +17853,11 @@
       <c r="L293" t="s">
         <v>17</v>
       </c>
-      <c r="M293" t="s">
-        <v>17</v>
+      <c r="M293">
+        <v>1167</v>
       </c>
       <c r="N293" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="294" spans="1:15" x14ac:dyDescent="0.2">
@@ -18073,11 +18073,11 @@
       <c r="L298" t="s">
         <v>17</v>
       </c>
-      <c r="M298" t="s">
-        <v>17</v>
+      <c r="M298">
+        <v>1655</v>
       </c>
       <c r="N298" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="299" spans="1:15" x14ac:dyDescent="0.2">
@@ -18117,11 +18117,11 @@
       <c r="L299" t="s">
         <v>17</v>
       </c>
-      <c r="M299" t="s">
-        <v>17</v>
+      <c r="M299">
+        <v>710</v>
       </c>
       <c r="N299" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="300" spans="1:15" x14ac:dyDescent="0.2">
@@ -18384,11 +18384,11 @@
       <c r="L305" t="s">
         <v>17</v>
       </c>
-      <c r="M305" t="s">
-        <v>17</v>
+      <c r="M305">
+        <v>1401</v>
       </c>
       <c r="N305" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="306" spans="1:15" x14ac:dyDescent="0.2">
@@ -18563,11 +18563,11 @@
       <c r="L309" t="s">
         <v>17</v>
       </c>
-      <c r="M309" t="s">
-        <v>17</v>
+      <c r="M309">
+        <v>866</v>
       </c>
       <c r="N309" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="310" spans="1:15" x14ac:dyDescent="0.2">
@@ -18695,11 +18695,11 @@
       <c r="L312" t="s">
         <v>17</v>
       </c>
-      <c r="M312" t="s">
-        <v>17</v>
+      <c r="M312">
+        <v>758</v>
       </c>
       <c r="N312" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="313" spans="1:15" x14ac:dyDescent="0.2">
@@ -19223,11 +19223,11 @@
       <c r="L324" t="s">
         <v>17</v>
       </c>
-      <c r="M324" t="s">
-        <v>17</v>
+      <c r="M324">
+        <v>1233</v>
       </c>
       <c r="N324" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="325" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>